<commit_message>
MFY auto commit at 02/02/2022 15:55:35
</commit_message>
<xml_diff>
--- a/Marks.xlsx
+++ b/Marks.xlsx
@@ -9,21 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="360" windowWidth="20490" windowHeight="7590"/>
+    <workbookView xWindow="0" yWindow="1080" windowWidth="20490" windowHeight="7590"/>
   </bookViews>
   <sheets>
-    <sheet name="SPM" sheetId="2" r:id="rId1"/>
-    <sheet name="SA" sheetId="3" r:id="rId2"/>
-    <sheet name="OS" sheetId="4" r:id="rId3"/>
-    <sheet name="POM" sheetId="5" r:id="rId4"/>
-    <sheet name="DCN" sheetId="6" r:id="rId5"/>
+    <sheet name="GPA" sheetId="7" r:id="rId1"/>
+    <sheet name="SPM" sheetId="2" r:id="rId2"/>
+    <sheet name="SA" sheetId="3" r:id="rId3"/>
+    <sheet name="OS" sheetId="4" r:id="rId4"/>
+    <sheet name="POM" sheetId="5" r:id="rId5"/>
+    <sheet name="DCN" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="24">
   <si>
     <t>Project</t>
   </si>
@@ -59,13 +60,49 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>Creadit hours</t>
+  </si>
+  <si>
+    <t>CGPA</t>
+  </si>
+  <si>
+    <t>Creadit Points</t>
+  </si>
+  <si>
+    <t>Grade Symbole</t>
+  </si>
+  <si>
+    <t>GPA</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>S_lab</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -87,6 +124,17 @@
       <color theme="0"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -115,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -123,10 +171,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -409,9 +466,191 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:J13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" style="5"/>
+    <col min="2" max="2" width="10.28515625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="5" customWidth="1"/>
+    <col min="4" max="16384" width="12.7109375" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C5" s="4"/>
+    </row>
+    <row r="7" spans="3:10" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="5" t="str">
+        <f>SPM!F14</f>
+        <v>A-</v>
+      </c>
+      <c r="E7" s="5" t="str">
+        <f>POM!F14</f>
+        <v>F</v>
+      </c>
+      <c r="F7" s="5" t="str">
+        <f>SA!F14</f>
+        <v>F</v>
+      </c>
+      <c r="G7" s="5" t="str">
+        <f>OS!F12</f>
+        <v>F</v>
+      </c>
+      <c r="H7" s="5" t="str">
+        <f>DCN!F12</f>
+        <v>F</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="5">
+        <f>IF(D7 = "A", 4, IF(D7 = "A-", 3.67, IF(D7 = "B+", 3.33, IF(D7 = "B", 3, IF(D7 = "B-", 2.67, IF(D7 = "C+", 2.33, IF(D7 = "C",2,  IF(D7 = "C-", 1.67, 0))))))))</f>
+        <v>3.67</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" ref="E8:I8" si="0">IF(E7 = "A", 4, IF(E7 = "A-", 3.67, IF(E7 = "B+", 3.33, IF(E7 = "B", 3, IF(E7 = "B-", 2.67, IF(E7 = "C+", 2.33, IF(E7 = "C",2,  IF(E7 = "C-", 1.67, 0))))))))</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J8" s="5">
+        <f>SUM(D8:I8)</f>
+        <v>7.67</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="5">
+        <v>3</v>
+      </c>
+      <c r="E9" s="5">
+        <v>3</v>
+      </c>
+      <c r="F9" s="5">
+        <v>3</v>
+      </c>
+      <c r="G9" s="5">
+        <v>3</v>
+      </c>
+      <c r="H9" s="5">
+        <v>3</v>
+      </c>
+      <c r="I9" s="5">
+        <v>3</v>
+      </c>
+      <c r="J9" s="5">
+        <f>SUM(D9:I9)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="5">
+        <f>D8*D9</f>
+        <v>11.01</v>
+      </c>
+      <c r="E10" s="5">
+        <f t="shared" ref="E10:I10" si="1">E8*E9</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="J10" s="5">
+        <f>SUM(D10:I10)</f>
+        <v>23.009999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="H12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="5">
+        <f>(J10/J9)</f>
+        <v>1.2783333333333333</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C13" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -425,12 +664,12 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="G4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="G4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
     </row>
     <row r="5" spans="2:10" ht="31.5" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
@@ -522,7 +761,7 @@
         <v>40</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" ref="E8:E12" si="0">(F9/D9)*C9</f>
+        <f t="shared" ref="E9:E12" si="0">(F9/D9)*C9</f>
         <v>9.75</v>
       </c>
       <c r="F9" s="2">
@@ -621,11 +860,11 @@
         <v>100</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <f>ROUND(SUM(E7:E12),2)</f>
         <v>84.58</v>
       </c>
-      <c r="F14" s="4" t="str">
+      <c r="F14" s="3" t="str">
         <f>IF(E14&gt;86,"A",IF(E14&gt;82,"A-",IF(E14&gt;78,"B+",IF(E14&gt;74,"B",IF(E14&gt;70,"B-",IF(E14&gt;66,"C+",IF(E14&gt;62,"C",IF(E14&gt;58,"C-","F"))))))))</f>
         <v>A-</v>
       </c>
@@ -643,12 +882,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -700,16 +939,20 @@
       <c r="C7" s="2">
         <v>15</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1" t="e">
+      <c r="D7" s="1">
+        <v>15</v>
+      </c>
+      <c r="E7" s="1">
         <f>(F7/D7)*C7</f>
-        <v>#DIV/0!</v>
+        <v>15</v>
       </c>
       <c r="F7" s="2">
         <f>SUM(G7:M7)</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="G7" s="1">
+        <v>15</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -721,18 +964,26 @@
       <c r="C8" s="2">
         <v>10</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1" t="e">
+      <c r="D8" s="1">
+        <v>30</v>
+      </c>
+      <c r="E8" s="1">
         <f>ROUND((F8/D8)*C8,2)</f>
-        <v>#DIV/0!</v>
+        <v>9</v>
       </c>
       <c r="F8" s="2">
         <f>SUM(G8:M8)</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="G8" s="1">
+        <v>10</v>
+      </c>
+      <c r="H8" s="1">
+        <v>8</v>
+      </c>
+      <c r="I8" s="1">
+        <v>9</v>
+      </c>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
@@ -742,16 +993,20 @@
       <c r="C9" s="2">
         <v>10</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1" t="e">
+      <c r="D9" s="1">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1">
         <f t="shared" ref="E9:E12" si="0">(F9/D9)*C9</f>
-        <v>#DIV/0!</v>
+        <v>10</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" ref="F9:F12" si="1">SUM(G9:M9)</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G9" s="1">
+        <v>10</v>
+      </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -763,10 +1018,12 @@
       <c r="C10" s="2">
         <v>40</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1" t="e">
+      <c r="D10" s="1">
+        <v>40</v>
+      </c>
+      <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="1"/>
@@ -784,16 +1041,20 @@
       <c r="C11" s="2">
         <v>20</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1" t="e">
+      <c r="D11" s="1">
+        <v>20</v>
+      </c>
+      <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>17.5</v>
       </c>
       <c r="F11" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="1"/>
+        <v>17.5</v>
+      </c>
+      <c r="G11" s="1">
+        <v>17.5</v>
+      </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -805,16 +1066,20 @@
       <c r="C12" s="2">
         <v>5</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1" t="e">
+      <c r="D12" s="1">
+        <v>5</v>
+      </c>
+      <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>5</v>
       </c>
       <c r="F12" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="G12" s="1">
+        <v>5</v>
+      </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -839,13 +1104,13 @@
         <v>100</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="2" t="e">
+      <c r="E14" s="2">
         <f>ROUND(SUM(E7:E12),2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F14" s="1" t="e">
+        <v>56.5</v>
+      </c>
+      <c r="F14" s="1" t="str">
         <f>IF(E14&gt;86,"A",IF(E14&gt;82,"A-",IF(E14&gt;78,"B+",IF(E14&gt;74,"B",IF(E14&gt;70,"B-",IF(E14&gt;66,"C+",IF(E14&gt;62,"C",IF(E14&gt;58,"C-","F"))))))))</f>
-        <v>#DIV/0!</v>
+        <v>F</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="1"/>
@@ -867,12 +1132,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:J15"/>
+  <dimension ref="B5:J60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:IV65536"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -919,66 +1184,78 @@
     </row>
     <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="2">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E7" s="1">
-        <f>(F7/D7)*C7</f>
-        <v>0</v>
+        <f>ROUND((F7/D7)*C7,2)</f>
+        <v>10</v>
       </c>
       <c r="F7" s="2">
         <f>SUM(G7:M7)</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G7" s="1">
+        <v>5</v>
+      </c>
+      <c r="H7" s="1">
+        <v>4</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="2">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E8" s="1">
-        <f>ROUND((F8/D8)*C8,2)</f>
-        <v>0</v>
+        <f t="shared" ref="E8:E10" si="0">(F8/D8)*C8</f>
+        <v>20</v>
       </c>
       <c r="F8" s="2">
-        <f>SUM(G8:M8)</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+        <f t="shared" ref="F8:F10" si="1">SUM(G8:M8)</f>
+        <v>94</v>
+      </c>
+      <c r="G8" s="1">
+        <v>52</v>
+      </c>
+      <c r="H8" s="1">
+        <v>34</v>
+      </c>
+      <c r="I8" s="1">
+        <v>8</v>
+      </c>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9" s="2">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D9" s="1">
-        <v>40</v>
+        <v>279</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" ref="E9:E12" si="0">(F9/D9)*C9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F9" s="2">
-        <f t="shared" ref="F9:F12" si="1">SUM(G9:M9)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G9" s="1"/>
@@ -988,13 +1265,231 @@
     </row>
     <row r="10" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1">
+        <v>112</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="0"/>
+        <v>15.178571428571427</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="G10" s="1">
+        <v>85</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2">
+        <f>SUM(C7:C10)</f>
+        <v>100</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2">
+        <f>ROUND(SUM(E7:E10),2)</f>
+        <v>45.18</v>
+      </c>
+      <c r="F12" s="1" t="str">
+        <f>IF(E12&gt;86,"A",IF(E12&gt;82,"A-",IF(E12&gt;78,"B+",IF(E12&gt;74,"B",IF(E12&gt;70,"B-",IF(E12&gt;66,"C+",IF(E12&gt;62,"C",IF(E12&gt;58,"C-","F"))))))))</f>
+        <v>F</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="60" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G60">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:K15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="256" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:11" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="B5" s="1"/>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2</v>
+      </c>
+      <c r="I5" s="2">
+        <v>3</v>
+      </c>
+      <c r="J5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1">
+        <v>15</v>
+      </c>
+      <c r="E7" s="1">
+        <f>(F7/D7)*C7</f>
+        <v>15</v>
+      </c>
+      <c r="F7" s="2">
+        <f>SUM(G7:M7)</f>
+        <v>15</v>
+      </c>
+      <c r="G7" s="1">
+        <v>15</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1">
+        <v>50</v>
+      </c>
+      <c r="E8" s="1">
+        <f>ROUND((F8/D8)*C8,2)</f>
+        <v>8</v>
+      </c>
+      <c r="F8" s="2">
+        <f>SUM(G8:M8)</f>
+        <v>40</v>
+      </c>
+      <c r="G8" s="1">
+        <v>10</v>
+      </c>
+      <c r="H8" s="1">
+        <v>8</v>
+      </c>
+      <c r="I8" s="1">
+        <v>7</v>
+      </c>
+      <c r="J8" s="1">
+        <v>8</v>
+      </c>
+      <c r="K8" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1">
+        <v>40</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" ref="E9:E12" si="0">(F9/D9)*C9</f>
+        <v>9.75</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" ref="F9:F12" si="1">SUM(G9:M9)</f>
+        <v>39</v>
+      </c>
+      <c r="G9" s="1">
+        <v>10</v>
+      </c>
+      <c r="H9" s="1">
+        <v>10</v>
+      </c>
+      <c r="I9" s="1">
+        <v>10</v>
+      </c>
+      <c r="J9" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B10" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="2">
         <v>40</v>
       </c>
       <c r="D10" s="1">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
@@ -1009,7 +1504,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
@@ -1021,18 +1516,20 @@
       </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="F11" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="G11" s="1">
+        <v>29</v>
+      </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
@@ -1044,18 +1541,20 @@
       </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F12" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="G12" s="1">
+        <v>5</v>
+      </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1066,7 +1565,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>11</v>
       </c>
@@ -1077,7 +1576,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2">
         <f>ROUND(SUM(E7:E12),2)</f>
-        <v>0</v>
+        <v>52.25</v>
       </c>
       <c r="F14" s="1" t="str">
         <f>IF(E14&gt;86,"A",IF(E14&gt;82,"A-",IF(E14&gt;78,"B+",IF(E14&gt;74,"B",IF(E14&gt;70,"B-",IF(E14&gt;66,"C+",IF(E14&gt;62,"C",IF(E14&gt;58,"C-","F"))))))))</f>
@@ -1088,7 +1587,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1103,12 +1602,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:J15"/>
+  <dimension ref="B5:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:IV65536"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1155,16 +1654,16 @@
     </row>
     <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="2">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E7" s="1">
-        <f>(F7/D7)*C7</f>
+        <f>ROUND((F7/D7)*C7,2)</f>
         <v>0</v>
       </c>
       <c r="F7" s="2">
@@ -1178,20 +1677,20 @@
     </row>
     <row r="8" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="2">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1">
-        <v>95</v>
+        <v>20</v>
       </c>
       <c r="E8" s="1">
-        <f>ROUND((F8/D8)*C8,2)</f>
+        <f t="shared" ref="E8:E10" si="0">(F8/D8)*C8</f>
         <v>0</v>
       </c>
       <c r="F8" s="2">
-        <f>SUM(G8:M8)</f>
+        <f t="shared" ref="F8:F10" si="1">SUM(G8:M8)</f>
         <v>0</v>
       </c>
       <c r="G8" s="1"/>
@@ -1201,20 +1700,20 @@
     </row>
     <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9" s="2">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D9" s="1">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" ref="E9:E12" si="0">(F9/D9)*C9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F9" s="2">
-        <f t="shared" ref="F9:F12" si="1">SUM(G9:M9)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G9" s="1"/>
@@ -1224,13 +1723,13 @@
     </row>
     <row r="10" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C10" s="2">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D10" s="1">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
@@ -1246,47 +1745,34 @@
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="2">
-        <v>20</v>
-      </c>
-      <c r="D11" s="1">
-        <v>40</v>
-      </c>
-      <c r="E11" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C12" s="2">
-        <v>5</v>
-      </c>
-      <c r="D12" s="1">
-        <v>5</v>
-      </c>
-      <c r="E12" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="1"/>
+        <f>SUM(C7:C10)</f>
+        <v>100</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2">
+        <f>ROUND(SUM(E7:E10),2)</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="1" t="str">
+        <f>IF(E12&gt;86,"A",IF(E12&gt;82,"A-",IF(E12&gt;78,"B+",IF(E12&gt;74,"B",IF(E12&gt;70,"B-",IF(E12&gt;66,"C+",IF(E12&gt;62,"C",IF(E12&gt;58,"C-","F"))))))))</f>
+        <v>F</v>
+      </c>
+      <c r="G12" s="2"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1295,280 +1781,11 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="2">
-        <f>SUM(C7:C12)</f>
-        <v>100</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2">
-        <f>ROUND(SUM(E7:E12),2)</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="1" t="str">
-        <f>IF(E14&gt;86,"A",IF(E14&gt;82,"A-",IF(E14&gt;78,"B+",IF(E14&gt;74,"B",IF(E14&gt;70,"B-",IF(E14&gt;66,"C+",IF(E14&gt;62,"C",IF(E14&gt;58,"C-","F"))))))))</f>
-        <v>F</v>
-      </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:J15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:IV65536"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="256" width="13.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="5" spans="2:10" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="2">
-        <v>1</v>
-      </c>
-      <c r="H5" s="2">
-        <v>2</v>
-      </c>
-      <c r="I5" s="2">
-        <v>3</v>
-      </c>
-      <c r="J5" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2">
-        <v>15</v>
-      </c>
-      <c r="D7" s="1">
-        <v>30</v>
-      </c>
-      <c r="E7" s="1">
-        <f>(F7/D7)*C7</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="2">
-        <f>SUM(G7:M7)</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2">
-        <v>10</v>
-      </c>
-      <c r="D8" s="1">
-        <v>95</v>
-      </c>
-      <c r="E8" s="1">
-        <f>ROUND((F8/D8)*C8,2)</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="2">
-        <f>SUM(G8:M8)</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="2">
-        <v>10</v>
-      </c>
-      <c r="D9" s="1">
-        <v>40</v>
-      </c>
-      <c r="E9" s="1">
-        <f t="shared" ref="E9:E12" si="0">(F9/D9)*C9</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="2">
-        <f t="shared" ref="F9:F12" si="1">SUM(G9:M9)</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2">
-        <v>40</v>
-      </c>
-      <c r="D10" s="1">
-        <v>100</v>
-      </c>
-      <c r="E10" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="2">
-        <v>20</v>
-      </c>
-      <c r="D11" s="1">
-        <v>40</v>
-      </c>
-      <c r="E11" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="2">
-        <v>5</v>
-      </c>
-      <c r="D12" s="1">
-        <v>5</v>
-      </c>
-      <c r="E12" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="2">
-        <f>SUM(C7:C12)</f>
-        <v>100</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2">
-        <f>ROUND(SUM(E7:E12),2)</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="1" t="str">
-        <f>IF(E14&gt;86,"A",IF(E14&gt;82,"A-",IF(E14&gt;78,"B+",IF(E14&gt;74,"B",IF(E14&gt;70,"B-",IF(E14&gt;66,"C+",IF(E14&gt;62,"C",IF(E14&gt;58,"C-","F"))))))))</f>
-        <v>F</v>
-      </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MFY auto commit at 02/02/2022 16:40:46
</commit_message>
<xml_diff>
--- a/Marks.xlsx
+++ b/Marks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1080" windowWidth="20490" windowHeight="7590"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="20490" windowHeight="7590"/>
   </bookViews>
   <sheets>
     <sheet name="GPA" sheetId="7" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="24">
   <si>
     <t>Project</t>
   </si>
@@ -468,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -525,7 +525,7 @@
       </c>
       <c r="G7" s="5" t="str">
         <f>OS!F12</f>
-        <v>F</v>
+        <v>B</v>
       </c>
       <c r="H7" s="5" t="str">
         <f>DCN!F12</f>
@@ -553,7 +553,7 @@
       </c>
       <c r="G8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H8" s="5">
         <f t="shared" si="0"/>
@@ -565,7 +565,7 @@
       </c>
       <c r="J8" s="5">
         <f>SUM(D8:I8)</f>
-        <v>7.67</v>
+        <v>10.67</v>
       </c>
     </row>
     <row r="9" spans="3:10" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -613,10 +613,10 @@
       </c>
       <c r="G10" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H10" s="5">
-        <f t="shared" si="1"/>
+        <f>H8*H9</f>
         <v>0</v>
       </c>
       <c r="I10" s="5">
@@ -625,7 +625,7 @@
       </c>
       <c r="J10" s="5">
         <f>SUM(D10:I10)</f>
-        <v>23.009999999999998</v>
+        <v>32.01</v>
       </c>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.2">
@@ -634,7 +634,7 @@
       </c>
       <c r="I12" s="5">
         <f>(J10/J9)</f>
-        <v>1.2783333333333333</v>
+        <v>1.7783333333333333</v>
       </c>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.2">
@@ -1137,7 +1137,7 @@
   <dimension ref="B5:J60"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1252,13 +1252,15 @@
       </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>30.107526881720432</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="1"/>
+        <v>210</v>
+      </c>
+      <c r="G9" s="1">
+        <v>210</v>
+      </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -1310,11 +1312,11 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2">
         <f>ROUND(SUM(E7:E10),2)</f>
-        <v>45.18</v>
+        <v>75.290000000000006</v>
       </c>
       <c r="F12" s="1" t="str">
         <f>IF(E12&gt;86,"A",IF(E12&gt;82,"A-",IF(E12&gt;78,"B+",IF(E12&gt;74,"B",IF(E12&gt;70,"B-",IF(E12&gt;66,"C+",IF(E12&gt;62,"C",IF(E12&gt;58,"C-","F"))))))))</f>
-        <v>F</v>
+        <v>B</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="1"/>
@@ -1346,7 +1348,7 @@
   <dimension ref="B5:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1396,21 +1398,21 @@
         <v>0</v>
       </c>
       <c r="C7" s="2">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E7" s="1">
         <f>(F7/D7)*C7</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F7" s="2">
         <f>SUM(G7:M7)</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G7" s="1">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -1428,26 +1430,26 @@
       </c>
       <c r="E8" s="1">
         <f>ROUND((F8/D8)*C8,2)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" s="2">
         <f>SUM(G8:M8)</f>
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G8" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H8" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I8" s="1">
         <v>7</v>
       </c>
       <c r="J8" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K8" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
@@ -1458,15 +1460,15 @@
         <v>10</v>
       </c>
       <c r="D9" s="1">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" ref="E9:E12" si="0">(F9/D9)*C9</f>
-        <v>9.75</v>
+        <f t="shared" ref="E9:E11" si="0">(F9/D9)*C9</f>
+        <v>10</v>
       </c>
       <c r="F9" s="2">
-        <f t="shared" ref="F9:F12" si="1">SUM(G9:M9)</f>
-        <v>39</v>
+        <f t="shared" ref="F9:F11" si="1">SUM(G9:M9)</f>
+        <v>50</v>
       </c>
       <c r="G9" s="1">
         <v>10</v>
@@ -1478,7 +1480,10 @@
         <v>10</v>
       </c>
       <c r="J9" s="1">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="K9" s="1">
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
@@ -1530,26 +1535,12 @@
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="2">
-        <v>5</v>
-      </c>
-      <c r="D12" s="1">
-        <v>5</v>
-      </c>
-      <c r="E12" s="1">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="F12" s="2">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="G12" s="1">
-        <v>5</v>
-      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1576,7 +1567,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2">
         <f>ROUND(SUM(E7:E12),2)</f>
-        <v>52.25</v>
+        <v>51.5</v>
       </c>
       <c r="F14" s="1" t="str">
         <f>IF(E14&gt;86,"A",IF(E14&gt;82,"A-",IF(E14&gt;78,"B+",IF(E14&gt;74,"B",IF(E14&gt;70,"B-",IF(E14&gt;66,"C+",IF(E14&gt;62,"C",IF(E14&gt;58,"C-","F"))))))))</f>

</xml_diff>

<commit_message>
MFY auto commit at 02/02/2022 19:12:46
</commit_message>
<xml_diff>
--- a/Marks.xlsx
+++ b/Marks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="20490" windowHeight="7590"/>
+    <workbookView xWindow="0" yWindow="2160" windowWidth="20490" windowHeight="7590" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="GPA" sheetId="7" r:id="rId1"/>
@@ -468,7 +468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10:I10"/>
     </sheetView>
   </sheetViews>
@@ -525,7 +525,7 @@
       </c>
       <c r="G7" s="5" t="str">
         <f>OS!F12</f>
-        <v>B</v>
+        <v>F</v>
       </c>
       <c r="H7" s="5" t="str">
         <f>DCN!F12</f>
@@ -553,7 +553,7 @@
       </c>
       <c r="G8" s="5">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H8" s="5">
         <f t="shared" si="0"/>
@@ -565,7 +565,7 @@
       </c>
       <c r="J8" s="5">
         <f>SUM(D8:I8)</f>
-        <v>10.67</v>
+        <v>7.67</v>
       </c>
     </row>
     <row r="9" spans="3:10" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -613,7 +613,7 @@
       </c>
       <c r="G10" s="5">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H10" s="5">
         <f>H8*H9</f>
@@ -625,7 +625,7 @@
       </c>
       <c r="J10" s="5">
         <f>SUM(D10:I10)</f>
-        <v>32.01</v>
+        <v>23.009999999999998</v>
       </c>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.2">
@@ -634,7 +634,7 @@
       </c>
       <c r="I12" s="5">
         <f>(J10/J9)</f>
-        <v>1.7783333333333333</v>
+        <v>1.2783333333333333</v>
       </c>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.2">
@@ -887,7 +887,7 @@
   <dimension ref="B5:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -965,15 +965,15 @@
         <v>10</v>
       </c>
       <c r="D8" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E8" s="1">
         <f>ROUND((F8/D8)*C8,2)</f>
-        <v>9</v>
+        <v>8.25</v>
       </c>
       <c r="F8" s="2">
         <f>SUM(G8:M8)</f>
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G8" s="1">
         <v>10</v>
@@ -982,9 +982,11 @@
         <v>8</v>
       </c>
       <c r="I8" s="1">
-        <v>9</v>
-      </c>
-      <c r="J8" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="J8" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
@@ -994,7 +996,7 @@
         <v>10</v>
       </c>
       <c r="D9" s="1">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" ref="E9:E12" si="0">(F9/D9)*C9</f>
@@ -1002,13 +1004,17 @@
       </c>
       <c r="F9" s="2">
         <f t="shared" ref="F9:F12" si="1">SUM(G9:M9)</f>
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G9" s="1">
         <v>10</v>
       </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="H9" s="1">
+        <v>10</v>
+      </c>
+      <c r="I9" s="1">
+        <v>10</v>
+      </c>
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
@@ -1106,7 +1112,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2">
         <f>ROUND(SUM(E7:E12),2)</f>
-        <v>56.5</v>
+        <v>55.75</v>
       </c>
       <c r="F14" s="1" t="str">
         <f>IF(E14&gt;86,"A",IF(E14&gt;82,"A-",IF(E14&gt;78,"B+",IF(E14&gt;74,"B",IF(E14&gt;70,"B-",IF(E14&gt;66,"C+",IF(E14&gt;62,"C",IF(E14&gt;58,"C-","F"))))))))</f>
@@ -1137,7 +1143,7 @@
   <dimension ref="B5:J60"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1252,15 +1258,13 @@
       </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>30.107526881720432</v>
+        <v>0</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="1"/>
-        <v>210</v>
-      </c>
-      <c r="G9" s="1">
-        <v>210</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -1312,11 +1316,11 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2">
         <f>ROUND(SUM(E7:E10),2)</f>
-        <v>75.290000000000006</v>
+        <v>45.18</v>
       </c>
       <c r="F12" s="1" t="str">
         <f>IF(E12&gt;86,"A",IF(E12&gt;82,"A-",IF(E12&gt;78,"B+",IF(E12&gt;74,"B",IF(E12&gt;70,"B-",IF(E12&gt;66,"C+",IF(E12&gt;62,"C",IF(E12&gt;58,"C-","F"))))))))</f>
-        <v>B</v>
+        <v>F</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="1"/>
@@ -1597,8 +1601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1655,13 +1659,15 @@
       </c>
       <c r="E7" s="1">
         <f>ROUND((F7/D7)*C7,2)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F7" s="2">
         <f>SUM(G7:M7)</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="G7" s="1">
+        <v>18</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -1678,13 +1684,15 @@
       </c>
       <c r="E8" s="1">
         <f t="shared" ref="E8:E10" si="0">(F8/D8)*C8</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" ref="F8:F10" si="1">SUM(G8:M8)</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="G8" s="1">
+        <v>18</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -1724,13 +1732,15 @@
       </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G10" s="1"/>
+        <v>85</v>
+      </c>
+      <c r="G10" s="1">
+        <v>85</v>
+      </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -1757,7 +1767,7 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2">
         <f>ROUND(SUM(E7:E10),2)</f>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="F12" s="1" t="str">
         <f>IF(E12&gt;86,"A",IF(E12&gt;82,"A-",IF(E12&gt;78,"B+",IF(E12&gt;74,"B",IF(E12&gt;70,"B-",IF(E12&gt;66,"C+",IF(E12&gt;62,"C",IF(E12&gt;58,"C-","F"))))))))</f>

</xml_diff>

<commit_message>
MFY auto commit at 02/02/2022 21:28:04
</commit_message>
<xml_diff>
--- a/Marks.xlsx
+++ b/Marks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2160" windowWidth="20490" windowHeight="7590" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="20490" windowHeight="7590"/>
   </bookViews>
   <sheets>
     <sheet name="GPA" sheetId="7" r:id="rId1"/>
@@ -468,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:I10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1143,7 +1143,7 @@
   <dimension ref="B5:J60"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1352,7 +1352,7 @@
   <dimension ref="B5:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1601,8 +1601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G7:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1659,15 +1659,13 @@
       </c>
       <c r="E7" s="1">
         <f>ROUND((F7/D7)*C7,2)</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F7" s="2">
         <f>SUM(G7:M7)</f>
-        <v>18</v>
-      </c>
-      <c r="G7" s="1">
-        <v>18</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -1684,15 +1682,13 @@
       </c>
       <c r="E8" s="1">
         <f t="shared" ref="E8:E10" si="0">(F8/D8)*C8</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" ref="F8:F10" si="1">SUM(G8:M8)</f>
-        <v>18</v>
-      </c>
-      <c r="G8" s="1">
-        <v>18</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -1732,15 +1728,13 @@
       </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
-      </c>
-      <c r="G10" s="1">
-        <v>85</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -1767,7 +1761,7 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2">
         <f>ROUND(SUM(E7:E10),2)</f>
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="F12" s="1" t="str">
         <f>IF(E12&gt;86,"A",IF(E12&gt;82,"A-",IF(E12&gt;78,"B+",IF(E12&gt;74,"B",IF(E12&gt;70,"B-",IF(E12&gt;66,"C+",IF(E12&gt;62,"C",IF(E12&gt;58,"C-","F"))))))))</f>

</xml_diff>

<commit_message>
MFY auto commit at 03/02/2022 17:51:09
</commit_message>
<xml_diff>
--- a/Marks.xlsx
+++ b/Marks.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="20490" windowHeight="7590"/>
+    <workbookView xWindow="0" yWindow="2880" windowWidth="20490" windowHeight="7590"/>
   </bookViews>
   <sheets>
     <sheet name="GPA" sheetId="7" r:id="rId1"/>
     <sheet name="SPM" sheetId="2" r:id="rId2"/>
-    <sheet name="SA" sheetId="3" r:id="rId3"/>
-    <sheet name="OS" sheetId="4" r:id="rId4"/>
-    <sheet name="POM" sheetId="5" r:id="rId5"/>
+    <sheet name="POM" sheetId="5" r:id="rId3"/>
+    <sheet name="SA" sheetId="3" r:id="rId4"/>
+    <sheet name="OS" sheetId="4" r:id="rId5"/>
     <sheet name="DCN" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -469,7 +469,7 @@
   <dimension ref="C4:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:I4"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -517,7 +517,7 @@
       </c>
       <c r="E7" s="5" t="str">
         <f>POM!F14</f>
-        <v>F</v>
+        <v>B+</v>
       </c>
       <c r="F7" s="5" t="str">
         <f>SA!F14</f>
@@ -545,18 +545,18 @@
       </c>
       <c r="E8" s="5">
         <f t="shared" ref="E8:I8" si="0">IF(E7 = "A", 4, IF(E7 = "A-", 3.67, IF(E7 = "B+", 3.33, IF(E7 = "B", 3, IF(E7 = "B-", 2.67, IF(E7 = "C+", 2.33, IF(E7 = "C",2,  IF(E7 = "C-", 1.67, 0))))))))</f>
-        <v>0</v>
+        <v>3.33</v>
       </c>
       <c r="F8" s="5">
-        <f t="shared" si="0"/>
+        <f>IF(F7 = "A", 4, IF(F7 = "A-", 3.67, IF(F7 = "B+", 3.33, IF(F7 = "B", 3, IF(F7 = "B-", 2.67, IF(F7 = "C+", 2.33, IF(F7 = "C",2,  IF(F7 = "C-", 1.67, 0))))))))</f>
         <v>0</v>
       </c>
       <c r="G8" s="5">
-        <f t="shared" si="0"/>
+        <f>IF(G7 = "A", 4, IF(G7 = "A-", 3.67, IF(G7 = "B+", 3.33, IF(G7 = "B", 3, IF(G7 = "B-", 2.67, IF(G7 = "C+", 2.33, IF(G7 = "C",2,  IF(G7 = "C-", 1.67, 0))))))))</f>
         <v>0</v>
       </c>
       <c r="H8" s="5">
-        <f t="shared" si="0"/>
+        <f>IF(H7 = "A", 4, IF(H7 = "A-", 3.67, IF(H7 = "B+", 3.33, IF(H7 = "B", 3, IF(H7 = "B-", 2.67, IF(H7 = "C+", 2.33, IF(H7 = "C",2,  IF(H7 = "C-", 1.67, 0))))))))</f>
         <v>0</v>
       </c>
       <c r="I8" s="5">
@@ -565,7 +565,7 @@
       </c>
       <c r="J8" s="5">
         <f>SUM(D8:I8)</f>
-        <v>7.67</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="3:10" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -605,14 +605,14 @@
       </c>
       <c r="E10" s="5">
         <f t="shared" ref="E10:I10" si="1">E8*E9</f>
-        <v>0</v>
+        <v>9.99</v>
       </c>
       <c r="F10" s="5">
-        <f t="shared" si="1"/>
+        <f>F8*F9</f>
         <v>0</v>
       </c>
       <c r="G10" s="5">
-        <f t="shared" si="1"/>
+        <f>G8*G9</f>
         <v>0</v>
       </c>
       <c r="H10" s="5">
@@ -625,7 +625,7 @@
       </c>
       <c r="J10" s="5">
         <f>SUM(D10:I10)</f>
-        <v>23.009999999999998</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.2">
@@ -634,7 +634,7 @@
       </c>
       <c r="I12" s="5">
         <f>(J10/J9)</f>
-        <v>1.2783333333333333</v>
+        <v>1.8333333333333333</v>
       </c>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.2">
@@ -884,6 +884,264 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:M15"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="256" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:13" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="B5" s="1"/>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2</v>
+      </c>
+      <c r="I5" s="2">
+        <v>3</v>
+      </c>
+      <c r="J5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="2:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1">
+        <v>20</v>
+      </c>
+      <c r="E7" s="1">
+        <f>(F7/D7)*C7</f>
+        <v>20</v>
+      </c>
+      <c r="F7" s="2">
+        <f>SUM(G7:M7)</f>
+        <v>20</v>
+      </c>
+      <c r="G7" s="1">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="2:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1">
+        <v>70</v>
+      </c>
+      <c r="E8" s="1">
+        <f>ROUND((F8/D8)*C8,2)</f>
+        <v>6.29</v>
+      </c>
+      <c r="F8" s="2">
+        <f>SUM(G8:M8)</f>
+        <v>44</v>
+      </c>
+      <c r="G8" s="1">
+        <v>8</v>
+      </c>
+      <c r="H8" s="1">
+        <v>7</v>
+      </c>
+      <c r="I8" s="1">
+        <v>7</v>
+      </c>
+      <c r="J8" s="1">
+        <v>7</v>
+      </c>
+      <c r="K8" s="1">
+        <v>6</v>
+      </c>
+      <c r="L8" s="1">
+        <v>5</v>
+      </c>
+      <c r="M8" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1">
+        <v>50</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" ref="E9:E11" si="0">(F9/D9)*C9</f>
+        <v>10</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" ref="F9:F11" si="1">SUM(G9:M9)</f>
+        <v>50</v>
+      </c>
+      <c r="G9" s="1">
+        <v>10</v>
+      </c>
+      <c r="H9" s="1">
+        <v>10</v>
+      </c>
+      <c r="I9" s="1">
+        <v>10</v>
+      </c>
+      <c r="J9" s="1">
+        <v>10</v>
+      </c>
+      <c r="K9" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2">
+        <v>40</v>
+      </c>
+      <c r="D10" s="1">
+        <v>60</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="G10" s="1">
+        <v>42</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="2:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2">
+        <v>20</v>
+      </c>
+      <c r="D11" s="1">
+        <v>40</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="0"/>
+        <v>14.5</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="G11" s="1">
+        <v>29</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="2:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="2:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="2:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="2">
+        <f>SUM(C7:C12)</f>
+        <v>100</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2">
+        <f>ROUND(SUM(E7:E12),2)</f>
+        <v>78.790000000000006</v>
+      </c>
+      <c r="F14" s="1" t="str">
+        <f>IF(E14&gt;86,"A",IF(E14&gt;82,"A-",IF(E14&gt;78,"B+",IF(E14&gt;74,"B",IF(E14&gt;70,"B-",IF(E14&gt;66,"C+",IF(E14&gt;62,"C",IF(E14&gt;58,"C-","F"))))))))</f>
+        <v>B+</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="2:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1138,7 +1396,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:J60"/>
   <sheetViews>
@@ -1341,256 +1599,6 @@
       <c r="G60">
         <v>0</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:K15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="256" width="13.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="5" spans="2:11" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="2">
-        <v>1</v>
-      </c>
-      <c r="H5" s="2">
-        <v>2</v>
-      </c>
-      <c r="I5" s="2">
-        <v>3</v>
-      </c>
-      <c r="J5" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2">
-        <v>20</v>
-      </c>
-      <c r="D7" s="1">
-        <v>20</v>
-      </c>
-      <c r="E7" s="1">
-        <f>(F7/D7)*C7</f>
-        <v>20</v>
-      </c>
-      <c r="F7" s="2">
-        <f>SUM(G7:M7)</f>
-        <v>20</v>
-      </c>
-      <c r="G7" s="1">
-        <v>20</v>
-      </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2">
-        <v>10</v>
-      </c>
-      <c r="D8" s="1">
-        <v>50</v>
-      </c>
-      <c r="E8" s="1">
-        <f>ROUND((F8/D8)*C8,2)</f>
-        <v>7</v>
-      </c>
-      <c r="F8" s="2">
-        <f>SUM(G8:M8)</f>
-        <v>35</v>
-      </c>
-      <c r="G8" s="1">
-        <v>8</v>
-      </c>
-      <c r="H8" s="1">
-        <v>7</v>
-      </c>
-      <c r="I8" s="1">
-        <v>7</v>
-      </c>
-      <c r="J8" s="1">
-        <v>7</v>
-      </c>
-      <c r="K8" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="2">
-        <v>10</v>
-      </c>
-      <c r="D9" s="1">
-        <v>50</v>
-      </c>
-      <c r="E9" s="1">
-        <f t="shared" ref="E9:E11" si="0">(F9/D9)*C9</f>
-        <v>10</v>
-      </c>
-      <c r="F9" s="2">
-        <f t="shared" ref="F9:F11" si="1">SUM(G9:M9)</f>
-        <v>50</v>
-      </c>
-      <c r="G9" s="1">
-        <v>10</v>
-      </c>
-      <c r="H9" s="1">
-        <v>10</v>
-      </c>
-      <c r="I9" s="1">
-        <v>10</v>
-      </c>
-      <c r="J9" s="1">
-        <v>10</v>
-      </c>
-      <c r="K9" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2">
-        <v>40</v>
-      </c>
-      <c r="D10" s="1">
-        <v>60</v>
-      </c>
-      <c r="E10" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="2">
-        <v>20</v>
-      </c>
-      <c r="D11" s="1">
-        <v>40</v>
-      </c>
-      <c r="E11" s="1">
-        <f t="shared" si="0"/>
-        <v>14.5</v>
-      </c>
-      <c r="F11" s="2">
-        <f t="shared" si="1"/>
-        <v>29</v>
-      </c>
-      <c r="G11" s="1">
-        <v>29</v>
-      </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="2">
-        <f>SUM(C7:C12)</f>
-        <v>100</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2">
-        <f>ROUND(SUM(E7:E12),2)</f>
-        <v>51.5</v>
-      </c>
-      <c r="F14" s="1" t="str">
-        <f>IF(E14&gt;86,"A",IF(E14&gt;82,"A-",IF(E14&gt;78,"B+",IF(E14&gt;74,"B",IF(E14&gt;70,"B-",IF(E14&gt;66,"C+",IF(E14&gt;62,"C",IF(E14&gt;58,"C-","F"))))))))</f>
-        <v>F</v>
-      </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>